<commit_message>
Add some indicators to Energy_balance.ipynb
</commit_message>
<xml_diff>
--- a/bilans2019.xlsx
+++ b/bilans2019.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ehlimana\Desktop\Load profiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ehlimana\Documents\GitHub\Electricity-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3182264-88C7-4B60-9536-27517291489E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988AC853-2765-4FAC-9DD8-36324FBAD4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{6F034462-F170-45F1-9CF6-4F6A972777C8}"/>
   </bookViews>
@@ -880,7 +880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2809EED2-E20C-47A0-B24E-8BE474AE50B9}">
   <dimension ref="A1:AM30"/>
   <sheetViews>
-    <sheetView topLeftCell="H25" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -998,7 +998,7 @@
         <v>10170</v>
       </c>
       <c r="L3" s="8">
-        <f t="shared" ref="L3:L8" si="0">SUM(B3:K3)</f>
+        <f t="shared" ref="L3:L6" si="0">SUM(B3:K3)</f>
         <v>131324</v>
       </c>
     </row>
@@ -1556,8 +1556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA27AC6-4A36-401F-80F6-18153FD4FB45}">
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView topLeftCell="F22" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4076,8 +4076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25F911DF-4B6F-441E-B6BD-B65E72F82DB7}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5711,8 +5711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6D149C9-3D44-465B-9C3F-638E8071DDE1}">
   <dimension ref="A1:R65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="N65" sqref="N65"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5779,10 +5779,10 @@
         <f>SUM(B2:K2)</f>
         <v>4741</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="1">
         <f>(G2+H2+I2)/L2</f>
         <v>0.25754060324825984</v>
       </c>
@@ -5810,10 +5810,10 @@
         <f>SUM(B3:K3)</f>
         <v>3430</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="1">
         <f>B2/L2</f>
         <v>0.74245939675174011</v>
       </c>
@@ -6011,9 +6011,10 @@
         <f>SUM(B12:K12)</f>
         <v>-27</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N12" s="1" t="s">
         <v>81</v>
       </c>
+      <c r="O12" s="1"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -6038,10 +6039,10 @@
         <f>SUM(B13:K13)</f>
         <v>-27</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N13" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="1">
         <f>(B11/(B11+D11+E11+G11+H11))*100</f>
         <v>86.288798920377857</v>
       </c>
@@ -6054,10 +6055,10 @@
         <f t="shared" ref="L14" si="3">SUM(B14:J14)</f>
         <v>0</v>
       </c>
-      <c r="N14" t="s">
+      <c r="N14" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="1">
         <f>(D11/(B11+D11+E11+G11+H11))*100</f>
         <v>0.37786774628879888</v>
       </c>
@@ -6076,10 +6077,10 @@
         <f t="shared" ref="L15:L16" si="4">SUM(B15:K15)</f>
         <v>-40</v>
       </c>
-      <c r="N15" t="s">
+      <c r="N15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="1">
         <f>(E11/(B11+D11+E11+G11+H11))*100</f>
         <v>0.18893387314439944</v>
       </c>
@@ -6095,10 +6096,10 @@
         <f t="shared" si="4"/>
         <v>-249</v>
       </c>
-      <c r="N16" t="s">
+      <c r="N16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="1">
         <f>(G11/(B11+D11+E11+H11+G11))*100</f>
         <v>13.090418353576247</v>
       </c>
@@ -6111,10 +6112,10 @@
         <f t="shared" ref="L17" si="5">SUM(B17:J17)</f>
         <v>0</v>
       </c>
-      <c r="N17" t="s">
+      <c r="N17" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="1">
         <f>(H11/(B11+D11+E11+G11+H11))*100</f>
         <v>5.3981106612685556E-2</v>
       </c>
@@ -6151,9 +6152,11 @@
         <f t="shared" si="6"/>
         <v>-423</v>
       </c>
-      <c r="N19" t="s">
+      <c r="N19" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
@@ -6175,10 +6178,12 @@
         <f t="shared" si="6"/>
         <v>-130</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="1">
         <f>(J11/(ABS(SUM(B11:H11))))*100</f>
         <v>40.728744939271252</v>
       </c>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
@@ -6228,10 +6233,11 @@
         <f>SUM(B21:K21)</f>
         <v>3606</v>
       </c>
-      <c r="N21" t="s">
+      <c r="N21" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="P21" t="s">
+      <c r="O21" s="1"/>
+      <c r="P21" s="1" t="s">
         <v>86</v>
       </c>
       <c r="R21" t="s">
@@ -6264,11 +6270,12 @@
         <f>SUM(B22:K22)</f>
         <v>754</v>
       </c>
-      <c r="N22">
+      <c r="N22" s="1">
         <f>(J12/ABS(B12))*100</f>
         <v>22.222222222222221</v>
       </c>
-      <c r="P22">
+      <c r="O22" s="1"/>
+      <c r="P22" s="1">
         <f>(K12/ABS(B12))*100</f>
         <v>44.444444444444443</v>
       </c>
@@ -6318,7 +6325,7 @@
         <f t="shared" si="8"/>
         <v>1140</v>
       </c>
-      <c r="N24" t="s">
+      <c r="N24" s="1" t="s">
         <v>88</v>
       </c>
     </row>
@@ -6348,7 +6355,7 @@
         <f t="shared" si="8"/>
         <v>435</v>
       </c>
-      <c r="N25">
+      <c r="N25" s="1">
         <f>(K13/ABS(B13+D13+E13+I13))*100</f>
         <v>78.571428571428569</v>
       </c>
@@ -6376,12 +6383,15 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N27" t="s">
+      <c r="N27" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1" t="s">
         <v>94</v>
       </c>
+      <c r="R27" s="1"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
@@ -6391,17 +6401,18 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N28" t="s">
+      <c r="N28" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="O28">
+      <c r="O28" s="1">
         <f>(B22/L22)*100</f>
         <v>26.127320954907162</v>
       </c>
-      <c r="Q28" t="s">
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="R28">
+      <c r="R28" s="1">
         <f>(B24/L24)*100</f>
         <v>6.4912280701754383</v>
       </c>
@@ -6417,17 +6428,18 @@
         <f t="shared" si="8"/>
         <v>75</v>
       </c>
-      <c r="N29" t="s">
+      <c r="N29" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="O29">
+      <c r="O29" s="1">
         <f>(D22/L22)*100</f>
         <v>14.854111405835543</v>
       </c>
-      <c r="Q29" t="s">
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="R29">
+      <c r="R29" s="1">
         <f>(D24/L24)*100</f>
         <v>7.3684210526315779</v>
       </c>
@@ -6477,49 +6489,52 @@
         <f t="shared" si="9"/>
         <v>3613</v>
       </c>
-      <c r="N30" t="s">
+      <c r="N30" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="O30">
+      <c r="O30" s="1">
         <f>(E22/L22)*100</f>
         <v>10.079575596816976</v>
       </c>
-      <c r="Q30" t="s">
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="R30">
+      <c r="R30" s="1">
         <f>(E24/L24)*100</f>
         <v>3.070175438596491</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="N31" t="s">
+      <c r="N31" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="O31">
+      <c r="O31" s="1">
         <f>(I22/L22)*100</f>
         <v>2.2546419098143233</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="R31">
+      <c r="R31" s="1">
         <f>(I24/L24)*100</f>
         <v>39.035087719298247</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="N32" t="s">
+      <c r="N32" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="O32">
+      <c r="O32" s="1">
         <f>(J22/L22)*100</f>
         <v>46.551724137931032</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="R32">
+      <c r="R32" s="1">
         <f>(J24/L24)*100</f>
         <v>35.701754385964911</v>
       </c>
@@ -6535,17 +6550,18 @@
       <c r="K33" t="s">
         <v>99</v>
       </c>
-      <c r="N33" t="s">
+      <c r="N33" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="O33">
+      <c r="O33" s="1">
         <f>(K22/L22)*100</f>
         <v>0.1326259946949602</v>
       </c>
-      <c r="Q33" t="s">
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="R33">
+      <c r="R33" s="1">
         <f>(K24/L24)*100</f>
         <v>8.3333333333333321</v>
       </c>
@@ -6558,6 +6574,11 @@
         <f>B19/L19</f>
         <v>0.3546099290780142</v>
       </c>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
     </row>
     <row r="35" spans="3:18" x14ac:dyDescent="0.35">
       <c r="J35" t="s">
@@ -6567,9 +6588,13 @@
         <f>D19/L19</f>
         <v>0.32624113475177308</v>
       </c>
-      <c r="N35" t="s">
+      <c r="N35" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
     </row>
     <row r="36" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C36" t="s">
@@ -6596,16 +6621,18 @@
         <f>J19/L19</f>
         <v>0.31678486997635935</v>
       </c>
-      <c r="N36" t="s">
+      <c r="N36" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="O36">
+      <c r="O36" s="1">
         <f>(B23/L23)*100</f>
         <v>0</v>
       </c>
-      <c r="Q36" t="s">
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="R36" s="1"/>
     </row>
     <row r="37" spans="3:18" x14ac:dyDescent="0.35">
       <c r="E37" t="s">
@@ -6625,17 +6652,18 @@
         <f>(K19/L19)</f>
         <v>2.3640661938534278E-3</v>
       </c>
-      <c r="N37" t="s">
+      <c r="N37" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="O37">
+      <c r="O37" s="1">
         <f>(D23/L23)*100</f>
         <v>99.496221662468514</v>
       </c>
-      <c r="Q37" t="s">
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="R37">
+      <c r="R37" s="1">
         <f>(B25/L25)*100</f>
         <v>25.057471264367813</v>
       </c>
@@ -6648,74 +6676,81 @@
         <f>100-F36</f>
         <v>68.107400130975776</v>
       </c>
-      <c r="N38" t="s">
+      <c r="N38" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="O38">
+      <c r="O38" s="1">
         <f>(E23/L23)*100</f>
         <v>0</v>
       </c>
-      <c r="Q38" t="s">
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="R38">
+      <c r="R38" s="1">
         <f>(D25/L25)*100</f>
         <v>11.724137931034482</v>
       </c>
     </row>
     <row r="39" spans="3:18" x14ac:dyDescent="0.35">
-      <c r="N39" t="s">
+      <c r="N39" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="O39">
+      <c r="O39" s="1">
         <f>(I23/L23)*100</f>
         <v>0</v>
       </c>
-      <c r="Q39" t="s">
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="R39">
+      <c r="R39" s="1">
         <f>(E25/L25)*100</f>
         <v>5.7471264367816088</v>
       </c>
     </row>
     <row r="40" spans="3:18" x14ac:dyDescent="0.35">
-      <c r="N40" t="s">
+      <c r="N40" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="O40">
+      <c r="O40" s="1">
         <f>(J23/L23)*100</f>
         <v>0.50377833753148615</v>
       </c>
-      <c r="Q40" t="s">
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="R40">
+      <c r="R40" s="1">
         <f>(I25/L25)*100</f>
         <v>8.2758620689655178</v>
       </c>
     </row>
     <row r="41" spans="3:18" x14ac:dyDescent="0.35">
-      <c r="N41" t="s">
+      <c r="N41" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="O41">
+      <c r="O41" s="1">
         <f>(K23/L23)*100</f>
         <v>0</v>
       </c>
-      <c r="Q41" t="s">
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="R41">
+      <c r="R41" s="1">
         <f>(J25/L25)*100</f>
         <v>42.298850574712645</v>
       </c>
     </row>
     <row r="42" spans="3:18" x14ac:dyDescent="0.35">
-      <c r="Q42" t="s">
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="R42">
+      <c r="R42" s="1">
         <f>(K25/L25)*100</f>
         <v>6.8965517241379306</v>
       </c>
@@ -6791,7 +6826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7406686-8E36-4D0C-83F1-B897A7E1F909}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="L22" sqref="L22:L24"/>
     </sheetView>
   </sheetViews>
@@ -8316,8 +8351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E415C40-8494-4F35-B83E-72693A09AC79}">
   <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+    <sheetView topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8327,6 +8362,7 @@
     <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="36.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">

</xml_diff>